<commit_message>
some initial analysis for EHR
</commit_message>
<xml_diff>
--- a/data/cotherapy/supp4_summary_drug_interactions.xlsx
+++ b/data/cotherapy/supp4_summary_drug_interactions.xlsx
@@ -55,7 +55,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Isoflurane,Calcium,Chlorpromazine</t>
+    <t>Chlorpromazine,Calcium,Isoflurane</t>
   </si>
   <si>
     <t>AKT1</t>
@@ -67,19 +67,19 @@
     <t>Activates</t>
   </si>
   <si>
-    <t>Alteplase,Tenecteplase,Reteplase,Tranexamic Acid|Alteplase,Tenecteplase,Reteplase,Tranexamic Acid</t>
-  </si>
-  <si>
-    <t>Ziprasidone,Pramipexole|Cabozantinib|Cabozantinib</t>
+    <t>Alteplase,Tranexamic Acid,Reteplase,Tenecteplase|Alteplase,Tranexamic Acid,Reteplase,Tenecteplase</t>
+  </si>
+  <si>
+    <t>Pramipexole,Ziprasidone|Cabozantinib|Cabozantinib</t>
   </si>
   <si>
     <t>Cabozantinib</t>
   </si>
   <si>
-    <t>Ziprasidone,Pramipexole|Tenecteplase,Alteplase,Reteplase</t>
-  </si>
-  <si>
-    <t>Ziprasidone,Pramipexole</t>
+    <t>Pramipexole,Ziprasidone|Alteplase,Reteplase,Tenecteplase</t>
+  </si>
+  <si>
+    <t>Pramipexole,Ziprasidone</t>
   </si>
   <si>
     <t>Cabozantinib|Ziprasidone|Ziprasidone</t>
@@ -160,10 +160,10 @@
     <t>Memantine</t>
   </si>
   <si>
-    <t>Memantine|Ziprasidone,Pergolide,Quetiapine,Aripiprazole,Imipramine,Nortriptyline</t>
-  </si>
-  <si>
-    <t>Memantine|Ziprasidone,Pergolide,Quetiapine,Aripiprazole,Imipramine,Nortriptyline|Ziprasidone,Pergolide,Quetiapine,Aripiprazole,Imipramine,Nortriptyline</t>
+    <t>Memantine|Ziprasidone,Quetiapine,Nortriptyline,Aripiprazole,Imipramine,Pergolide</t>
+  </si>
+  <si>
+    <t>Memantine|Ziprasidone,Quetiapine,Nortriptyline,Aripiprazole,Imipramine,Pergolide|Ziprasidone,Quetiapine,Nortriptyline,Aripiprazole,Imipramine,Pergolide</t>
   </si>
   <si>
     <t>CALM3,HRH4</t>
@@ -256,7 +256,7 @@
     <t>Decreased levels of Favtor VII associated with DVT</t>
   </si>
   <si>
-    <t>Eprosartan,Telmisartan,Olmesartan,Desmopressin,Carvedilol,Irbesartan</t>
+    <t>Olmesartan,Telmisartan,Irbesartan,Eprosartan,Desmopressin,Carvedilol</t>
   </si>
   <si>
     <t>Aminocaproic Acid</t>
@@ -304,19 +304,19 @@
     <t>Low levels of plasmin associated with edema</t>
   </si>
   <si>
-    <t>Ibuprofen,Thalidomide,Nabumetone,Caffeine,Meloxicam</t>
-  </si>
-  <si>
-    <t>Hyoscyamine,Atropine,Scopolamine,Clozapine,Paroxetine|Hyoscyamine,Atropine,Ropinirole,Cabergoline,Scopolamine,Clozapine,Paroxetine,Caffeine,Pramipexole,Diphenhydramine</t>
-  </si>
-  <si>
-    <t>Metoprolol,Ropinirole,Cabergoline,Clozapine,Pseudoephedrine,Caffeine,Pramipexole</t>
-  </si>
-  <si>
-    <t>Hyoscyamine,Atropine,Ropinirole,Cabergoline,Scopolamine,Clozapine,Paroxetine,Caffeine,Pramipexole,Diphenhydramine|Cabergoline</t>
-  </si>
-  <si>
-    <t>Hyoscyamine,Metoprolol,Ibuprofen,Atropine,Cabergoline,Scopolamine,Thalidomide,Clozapine,Lidocaine,Paroxetine,Pseudoephedrine,Caffeine,Diphenhydramine|Nilotinib,Thalidomide,Imatinib,Lidocaine,Caffeine</t>
+    <t>Caffeine,Meloxicam,Thalidomide,Nabumetone,Ibuprofen</t>
+  </si>
+  <si>
+    <t>Hyoscyamine,Paroxetine,Atropine,Scopolamine,Clozapine|Pramipexole,Cabergoline,Caffeine,Diphenhydramine,Hyoscyamine,Paroxetine,Atropine,Scopolamine,Ropinirole,Clozapine</t>
+  </si>
+  <si>
+    <t>Pramipexole,Cabergoline,Caffeine,Pseudoephedrine,Ropinirole,Clozapine,Metoprolol</t>
+  </si>
+  <si>
+    <t>Pramipexole,Cabergoline,Caffeine,Diphenhydramine,Hyoscyamine,Paroxetine,Atropine,Scopolamine,Ropinirole,Clozapine|Cabergoline</t>
+  </si>
+  <si>
+    <t>Cabergoline,Diphenhydramine,Caffeine,Hyoscyamine,Thalidomide,Paroxetine,Ibuprofen,Atropine,Scopolamine,Lidocaine,Pseudoephedrine,Clozapine,Metoprolol|Caffeine,Imatinib,Thalidomide,Nilotinib,Lidocaine</t>
   </si>
   <si>
     <t>TP53</t>
@@ -364,43 +364,43 @@
     <t>histamine receptor antagonists prevent gastric ulcers</t>
   </si>
   <si>
-    <t>Glucosamine,Auranofin</t>
-  </si>
-  <si>
-    <t>Mefenamic acid,Etanercept,Piroxicam,Thalidomide,Bromfenac,Ketoprofen,Nabumetone,Oxaprozin,Fenoprofen,Meloxicam,Meclofenamic acid,Tolmetin|Auranofin</t>
+    <t>Auranofin,Glucosamine</t>
+  </si>
+  <si>
+    <t>Bromfenac,Mefenamic acid,Meloxicam,Thalidomide,Piroxicam,Tolmetin,Nabumetone,Oxaprozin,Ketoprofen,Fenoprofen,Etanercept,Meclofenamic acid|Auranofin</t>
   </si>
   <si>
     <t>Quinine</t>
   </si>
   <si>
-    <t>Fondaparinux sodium,Cephalexin,Ampicillin,Heparin,Lauric Acid,Desflurane,Tacrolimus,Edoxaban,Cefotetan,Tetracycline,Hyaluronidase,Methyltestosterone,Ceftriaxone,Cefotaxime,Oxymetholone,Clonazepam,Acitretin,Methotrexate,Vancomycin,Vandetanib,Sevoflurane,Naproxen,Enoxaparin,Cefazolin,Fosphenytoin,Ketoprofen,Rivaroxaban,Flurbiprofen,Bismuth Subsalicylate,Auranofin,Piroxicam,Prednisone,Salicylic acid,Fenoprofen,Diflunisal</t>
-  </si>
-  <si>
-    <t>Ketoprofen,Quetiapine,Olanzapine,Aripiprazole</t>
-  </si>
-  <si>
-    <t>Aripiprazole,Risperidone,Epinephrine,Quetiapine,Olanzapine,Carvedilol|Ampicillin,Prasugrel,Lauric Acid,Risperidone,Tacrolimus,Cefotetan,Iloprost,Tetracycline,Hyaluronidase,Diazoxide,Clonazepam,Pentoxifylline,Epinephrine,Carvedilol,Vancomycin,Vandetanib,Ketoprofen,Quetiapine,Olanzapine,Aripiprazole,Bismuth Subsalicylate,Auranofin,Phenylephrine,Fenoprofen</t>
-  </si>
-  <si>
-    <t>Quetiapine,Olanzapine,Aripiprazole|Phenylephrine,Bivalirudin,Risperidone,Epinephrine,Quetiapine,Goserelin,Carvedilol,Aripiprazole,Olanzapine|Quetiapine,Olanzapine,Aripiprazole</t>
-  </si>
-  <si>
-    <t>Quinine|Fondaparinux sodium,Cephalexin,Ampicillin,Heparin,Lauric Acid,Desflurane,Tacrolimus,Edoxaban,Cefotetan,Tetracycline,Hyaluronidase,Methyltestosterone,Ceftriaxone,Cefotaxime,Oxymetholone,Clonazepam,Acitretin,Methotrexate,Vancomycin,Vandetanib,Sevoflurane,Naproxen,Enoxaparin,Cefazolin,Fosphenytoin,Ketoprofen,Rivaroxaban,Flurbiprofen,Bismuth Subsalicylate,Auranofin,Piroxicam,Prednisone,Salicylic acid,Fenoprofen,Diflunisal</t>
-  </si>
-  <si>
-    <t>Tenecteplase,Alteplase,Reteplase,Aprotinin</t>
-  </si>
-  <si>
-    <t>Thalidomide,Pazopanib,Ponatinib,Sorafenib,Regorafenib,Dasatinib</t>
-  </si>
-  <si>
-    <t>Tenecteplase,Alteplase,Eptifibatide,Abciximab,Tirofiban,Ponatinib,Reteplase,Nintedanib,Dasatinib|Tenecteplase,Alteplase,Eptifibatide,Abciximab,Tirofiban,Ponatinib,Reteplase,Nintedanib,Dasatinib|Thalidomide,Pazopanib,Ponatinib,Sorafenib,Regorafenib,Dasatinib</t>
-  </si>
-  <si>
-    <t>Dabigatran etexilate,Sevoflurane,Desflurane,Bivalirudin,Methotrexate</t>
-  </si>
-  <si>
-    <t>Prasugrel,Risperidone,Pentoxifylline,Ketoprofen,Quetiapine,Olanzapine,Aripiprazole</t>
+    <t>Flurbiprofen,Piroxicam,Hyaluronidase,Methyltestosterone,Heparin,Prednisone,Diflunisal,Cefazolin,Vancomycin,Cefotaxime,Tacrolimus,Vandetanib,Cephalexin,Naproxen,Fosphenytoin,Salicylic acid,Oxymetholone,Sevoflurane,Fondaparinux sodium,Lauric Acid,Bismuth Subsalicylate,Edoxaban,Ketoprofen,Fenoprofen,Ceftriaxone,Acitretin,Ampicillin,Rivaroxaban,Clonazepam,Cefotetan,Tetracycline,Desflurane,Methotrexate,Enoxaparin,Auranofin</t>
+  </si>
+  <si>
+    <t>Aripiprazole,Olanzapine,Quetiapine,Ketoprofen</t>
+  </si>
+  <si>
+    <t>Quetiapine,Aripiprazole,Risperidone,Olanzapine,Epinephrine,Carvedilol|Hyaluronidase,Pentoxifylline,Iloprost,Vancomycin,Quetiapine,Tacrolimus,Olanzapine,Phenylephrine,Prasugrel,Vandetanib,Carvedilol,Diazoxide,Lauric Acid,Bismuth Subsalicylate,Aripiprazole,Risperidone,Epinephrine,Ketoprofen,Fenoprofen,Ampicillin,Clonazepam,Cefotetan,Tetracycline,Auranofin</t>
+  </si>
+  <si>
+    <t>Aripiprazole,Olanzapine,Quetiapine|Quetiapine,Aripiprazole,Risperidone,Olanzapine,Phenylephrine,Epinephrine,Goserelin,Carvedilol,Bivalirudin|Aripiprazole,Olanzapine,Quetiapine</t>
+  </si>
+  <si>
+    <t>Quinine|Flurbiprofen,Piroxicam,Hyaluronidase,Methyltestosterone,Heparin,Prednisone,Diflunisal,Cefazolin,Vancomycin,Cefotaxime,Tacrolimus,Vandetanib,Cephalexin,Naproxen,Fosphenytoin,Salicylic acid,Oxymetholone,Sevoflurane,Fondaparinux sodium,Lauric Acid,Bismuth Subsalicylate,Edoxaban,Ketoprofen,Fenoprofen,Ceftriaxone,Acitretin,Ampicillin,Rivaroxaban,Clonazepam,Cefotetan,Tetracycline,Desflurane,Methotrexate,Enoxaparin,Auranofin</t>
+  </si>
+  <si>
+    <t>Alteplase,Reteplase,Tenecteplase,Aprotinin</t>
+  </si>
+  <si>
+    <t>Pazopanib,Dasatinib,Thalidomide,Ponatinib,Sorafenib,Regorafenib</t>
+  </si>
+  <si>
+    <t>Nintedanib,Dasatinib,Tirofiban,Ponatinib,Abciximab,Tenecteplase,Eptifibatide,Reteplase,Alteplase|Nintedanib,Dasatinib,Tirofiban,Ponatinib,Abciximab,Tenecteplase,Eptifibatide,Reteplase,Alteplase|Pazopanib,Dasatinib,Thalidomide,Ponatinib,Sorafenib,Regorafenib</t>
+  </si>
+  <si>
+    <t>Sevoflurane,Desflurane,Bivalirudin,Methotrexate,Dabigatran etexilate</t>
+  </si>
+  <si>
+    <t>Quetiapine,Aripiprazole,Risperidone,Olanzapine,Pentoxifylline,Prasugrel,Ketoprofen</t>
   </si>
   <si>
     <t>CHUK</t>
@@ -607,28 +607,28 @@
     <t>Reduced clinically-relevant bleeding compared to Warfarin</t>
   </si>
   <si>
-    <t>Pimozide,Promethazine,Fluphenazine,Perphenazine,Vandetanib|Iloprost</t>
-  </si>
-  <si>
-    <t>Ziprasidone,Clozapine,Loxapine,Tramadol,Degarelix,Conivaptan,Amitriptyline,Bromocriptine,Dextroamphetamine,Maprotiline,Paliperidone,Solifenacin,Cyclobenzaprine,Lurasidone,Doxepin,Phenylephrine,Pergolide,Trihexyphenidyl,Ipratropium bromide,Terazosin,Leuprolide,Ropinirole,Oxymetazoline,Cyclopentolate,Darifenacin,Haloperidol,Cabergoline,Cetirizine,Clonidine,Naphazoline,Propantheline,Histamine,Escitalopram,Losartan,Asenapine,Clemastine,Nortriptyline,Desipramine,Hyoscyamine,Bivalirudin,Risperidone,Protirelin,Eletriptan,Isometheptene,Amoxapine,Epinephrine,Cevimeline,Tiotropium,Dihydroergotamine,Dexamethasone,Droperidol,Ergotamine,Carbinoxamine,Paroxetine,Cinacalcet,Succinylcholine,Diphenhydramine,Pramipexole,Atropine,Donepezil,Brompheniramine,Apraclonidine,Modafinil,Goserelin,Triprolidine,Lisdexamfetamine,Pilocarpine,Acamprosate,Phentolamine,Citalopram,Triptorelin,Droxidopa,Midodrine,Imipramine,Ephedrine,Scopolamine,Trazodone,Metoclopramide,Nefazodone,Quetiapine,Dicyclomine,Mirtazapine,Pseudoephedrine,Olanzapine,Aripiprazole,Cyproheptadine,Azelastine,Trimipramine,Promethazine,Oxybutynin|Ziprasidone,Clozapine,Loxapine,Tramadol,Degarelix,Conivaptan,Amitriptyline,Bromocriptine,Dextroamphetamine,Maprotiline,Paliperidone,Solifenacin,Cyclobenzaprine,Lurasidone,Doxepin,Phenylephrine,Pergolide,Trihexyphenidyl,Ipratropium bromide,Terazosin,Leuprolide,Oxymetazoline,Ropinirole,Cyclopentolate,Darifenacin,Haloperidol,Cabergoline,Cetirizine,Clonidine,Naphazoline,Propantheline,Histamine,Escitalopram,Losartan,Asenapine,Clemastine,Nortriptyline,Desipramine,Hyoscyamine,Bivalirudin,Risperidone,Protirelin,Eletriptan,Isometheptene,Amoxapine,Epinephrine,Cevimeline,Tiotropium,Dihydroergotamine,Dexamethasone,Droperidol,Ergotamine,Carbinoxamine,Paroxetine,Cinacalcet,Diphenhydramine,Succinylcholine,Pramipexole,Atropine,Donepezil,Brompheniramine,Apraclonidine,Modafinil,Goserelin,Lisdexamfetamine,Triprolidine,Pilocarpine,Acamprosate,Phentolamine,Triptorelin,Citalopram,Droxidopa,Midodrine,Imipramine,Ephedrine,Scopolamine,Trazodone,Metoclopramide,Nefazodone,Quetiapine,Dicyclomine,Olanzapine,Pseudoephedrine,Mirtazapine,Aripiprazole,Cyproheptadine,Azelastine,Trimipramine,Promethazine,Oxybutynin</t>
-  </si>
-  <si>
-    <t>Tenecteplase,Nintedanib</t>
-  </si>
-  <si>
-    <t>Ziprasidone,Almotriptan,Ondansetron,Modafinil,Rotigotine,Clozapine,Progesterone,Epinephrine,Citalopram,Amitriptyline,Imipramine,Clonidine,Pimozide,Olanzapine,Cyclobenzaprine,Perphenazine,Cinacalcet,Azelastine,Losartan,Propranolol,Asenapine,Desipramine|Ziprasidone,Almotriptan,Ondansetron,Modafinil,Rotigotine,Clozapine,Progesterone,Epinephrine,Citalopram,Amitriptyline,Imipramine,Clonidine,Pimozide,Olanzapine,Cyclobenzaprine,Perphenazine,Cinacalcet,Azelastine,Losartan,Propranolol,Asenapine,Desipramine|Ketamine,Ziprasidone,Almotriptan,Ondansetron,Modafinil,Rotigotine,Clozapine,Fluphenazine,Salmeterol,Tramadol,Buspirone,Dopamine,Zolmitriptan,Frovatriptan,Darifenacin,Eletriptan,Sufentanil,Progesterone,Conivaptan,Epinephrine,Citalopram,Hydrocodone,Cevimeline,Tiotropium,Amitriptyline,Imipramine,Fentanyl,Hydromorphone,Oxycodone,Codeine,Dexamethasone,Clonidine,Rizatriptan,Pimozide,Brompheniramine,Trazodone,Carbinoxamine,Paroxetine,Quetiapine,Dronabinol,Dextromethorphan,Olanzapine,Aripiprazole,Cyclobenzaprine,Perphenazine,Cinacalcet,Diphenhydramine,Tizanidine,Histamine,Escitalopram,Mirabegron,Donepezil,Azelastine,Losartan,Phenylephrine,Propranolol,Oxymorphone,Asenapine,Ticagrelor,Oxybutynin,Clemastine,Morphine,Desipramine,Ipratropium bromide</t>
-  </si>
-  <si>
-    <t>Ziprasidone,Terazosin,Modafinil,Oxymetazoline,Clozapine,Loxapine,Iloprost,Lisdexamfetamine,Cabergoline,Epinephrine,Amitriptyline,Bromocriptine,Midodrine,Imipramine,Droxidopa,Clonidine,Ergotamine,Dextroamphetamine,Nefazodone,Quetiapine,Paliperidone,Olanzapine,Aripiprazole,Doxepin,Mirabegron,Phenylephrine,Trimipramine,Losartan,Nortriptyline</t>
-  </si>
-  <si>
-    <t>Amitriptyline,Losartan,Olanzapine,Mirabegron</t>
-  </si>
-  <si>
-    <t>Ziprasidone,Terazosin,Apraclonidine,Leuprolide,Modafinil,Ropinirole,Clozapine,Loxapine,Tramadol,Degarelix,Cyclopentolate,Triprolidine,Darifenacin,Lisdexamfetamine,Protirelin,Eletriptan,Isometheptene,Acamprosate,Phentolamine,Conivaptan,Cabergoline,Amoxapine,Epinephrine,Citalopram,Triptorelin,Cevimeline,Amitriptyline,Tiotropium,Imipramine,Bromocriptine,Brompheniramine,Midodrine,Cetirizine,Clonidine,Droperidol,Scopolamine,Ergotamine,Ephedrine,Naphazoline,Propantheline,Trazodone,Dextroamphetamine,Maprotiline,Paroxetine,Quetiapine,Nefazodone,Paliperidone,Mirtazapine,Olanzapine,Cyclobenzaprine,Aripiprazole,Pseudoephedrine,Pramipexole,Diphenhydramine,Cinacalcet,Histamine,Cyproheptadine,Doxepin,Escitalopram,Donepezil,Azelastine,Trimipramine,Losartan,Phenylephrine,Carbinoxamine,Promethazine,Asenapine,Pergolide,Oxybutynin,Clemastine,Nortriptyline,Desipramine,Ipratropium bromide|Ziprasidone,Terazosin,Apraclonidine,Leuprolide,Modafinil,Ropinirole,Bivalirudin,Clozapine,Loxapine,Tramadol,Degarelix,Cyclopentolate,Triprolidine,Darifenacin,Lisdexamfetamine,Protirelin,Eletriptan,Isometheptene,Acamprosate,Phentolamine,Conivaptan,Cabergoline,Amoxapine,Epinephrine,Citalopram,Triptorelin,Cevimeline,Amitriptyline,Tiotropium,Imipramine,Bromocriptine,Brompheniramine,Midodrine,Cetirizine,Dexamethasone,Clonidine,Droperidol,Scopolamine,Ergotamine,Ephedrine,Naphazoline,Propantheline,Trazodone,Dextroamphetamine,Maprotiline,Paroxetine,Quetiapine,Nefazodone,Paliperidone,Mirtazapine,Olanzapine,Cyclobenzaprine,Aripiprazole,Pseudoephedrine,Pramipexole,Diphenhydramine,Cinacalcet,Histamine,Cyproheptadine,Doxepin,Escitalopram,Donepezil,Azelastine,Trimipramine,Losartan,Phenylephrine,Carbinoxamine,Promethazine,Asenapine,Pergolide,Oxybutynin,Clemastine,Nortriptyline,Desipramine,Ipratropium bromide</t>
-  </si>
-  <si>
-    <t>Ziprasidone,Rotigotine,Regadenoson,Ondansetron,Ropinirole,Mefloquine,Timolol,Clozapine,Fluphenazine,Salmeterol,Loxapine,Iloprost,Methamphetamine,Dopamine,Adenosine,Haloperidol,Eletriptan,Indacaterol,Metoprolol,Teriparatide,Conivaptan,Levodopa,Cabergoline,Amphetamine,Amoxapine,Epinephrine,Tesamorelin,Amitriptyline,Bromocriptine,Droxidopa,Imipramine,Terbutaline,Arformoterol,Metipranolol,Sotalol,Dextroamphetamine,Maprotiline,Metoclopramide,Quetiapine,Paliperidone,Olanzapine,Aripiprazole,Pseudoephedrine,Mirtazapine,Lurasidone,Perphenazine,Pramipexole,Histamine,Formoterol,Doxepin,Mirabegron,Propranolol,Asenapine,Famotidine,Nortriptyline,Ranitidine,Desipramine|Ziprasidone,Clozapine,Loxapine,Tramadol,Degarelix,Conivaptan,Amitriptyline,Bromocriptine,Dextroamphetamine,Maprotiline,Paliperidone,Solifenacin,Cyclobenzaprine,Lurasidone,Doxepin,Phenylephrine,Pergolide,Ipratropium bromide,Terazosin,Leuprolide,Ropinirole,Oxymetazoline,Cyclopentolate,Darifenacin,Haloperidol,Cabergoline,Cetirizine,Clonidine,Naphazoline,Propantheline,Histamine,Escitalopram,Losartan,Asenapine,Clemastine,Nortriptyline,Desipramine,Hyoscyamine,Bivalirudin,Protirelin,Eletriptan,Isometheptene,Amoxapine,Epinephrine,Cevimeline,Tiotropium,Dihydroergotamine,Dexamethasone,Droperidol,Ergotamine,Carbinoxamine,Paroxetine,Pramipexole,Diphenhydramine,Succinylcholine,Cinacalcet,Atropine,Donepezil,Brompheniramine,Apraclonidine,Modafinil,Lisdexamfetamine,Triprolidine,Pilocarpine,Acamprosate,Phentolamine,Citalopram,Triptorelin,Droxidopa,Midodrine,Imipramine,Ephedrine,Scopolamine,Trazodone,Nefazodone,Metoclopramide,Quetiapine,Dicyclomine,Mirtazapine,Olanzapine,Aripiprazole,Pseudoephedrine,Cyproheptadine,Azelastine,Trimipramine,Promethazine,Oxybutynin</t>
+    <t>Pimozide,Promethazine,Perphenazine,Vandetanib,Fluphenazine|Iloprost</t>
+  </si>
+  <si>
+    <t>Cinacalcet,Cevimeline,Midodrine,Goserelin,Apraclonidine,Ephedrine,Protirelin,Cyclobenzaprine,Oxybutynin,Clemastine,Succinylcholine,Trazodone,Epinephrine,Paroxetine,Bromocriptine,Ropinirole,Bivalirudin,Carbinoxamine,Citalopram,Amoxapine,Eletriptan,Pseudoephedrine,Mirtazapine,Losartan,Quetiapine,Isometheptene,Olanzapine,Phenylephrine,Loxapine,Paliperidone,Conivaptan,Pramipexole,Escitalopram,Aripiprazole,Nefazodone,Naphazoline,Phentolamine,Droperidol,Clonidine,Clozapine,Dicyclomine,Propantheline,Pilocarpine,Tiotropium,Trihexyphenidyl,Azelastine,Cyproheptadine,Cetirizine,Diphenhydramine,Acamprosate,Triprolidine,Promethazine,Leuprolide,Tramadol,Amitriptyline,Hyoscyamine,Scopolamine,Metoclopramide,Ergotamine,Asenapine,Oxymetazoline,Donepezil,Terazosin,Trimipramine,Solifenacin,Ipratropium bromide,Haloperidol,Cabergoline,Cyclopentolate,Triptorelin,Histamine,Degarelix,Droxidopa,Brompheniramine,Nortriptyline,Pergolide,Lurasidone,Dexamethasone,Risperidone,Dihydroergotamine,Desipramine,Darifenacin,Atropine,Lisdexamfetamine,Ziprasidone,Dextroamphetamine,Doxepin,Imipramine,Maprotiline,Modafinil|Cinacalcet,Cevimeline,Midodrine,Goserelin,Apraclonidine,Ephedrine,Cyclobenzaprine,Protirelin,Oxybutynin,Clemastine,Succinylcholine,Trazodone,Epinephrine,Paroxetine,Bromocriptine,Ropinirole,Bivalirudin,Carbinoxamine,Citalopram,Amoxapine,Eletriptan,Pseudoephedrine,Mirtazapine,Quetiapine,Losartan,Isometheptene,Olanzapine,Loxapine,Phenylephrine,Paliperidone,Conivaptan,Pramipexole,Escitalopram,Aripiprazole,Nefazodone,Naphazoline,Phentolamine,Droperidol,Clonidine,Clozapine,Dicyclomine,Propantheline,Pilocarpine,Tiotropium,Trihexyphenidyl,Azelastine,Cyproheptadine,Cetirizine,Diphenhydramine,Acamprosate,Triprolidine,Promethazine,Leuprolide,Tramadol,Amitriptyline,Hyoscyamine,Scopolamine,Metoclopramide,Ergotamine,Asenapine,Oxymetazoline,Donepezil,Terazosin,Trimipramine,Solifenacin,Ipratropium bromide,Haloperidol,Cabergoline,Cyclopentolate,Triptorelin,Histamine,Degarelix,Droxidopa,Brompheniramine,Nortriptyline,Pergolide,Lurasidone,Dexamethasone,Risperidone,Dihydroergotamine,Desipramine,Darifenacin,Atropine,Lisdexamfetamine,Ziprasidone,Dextroamphetamine,Doxepin,Imipramine,Maprotiline,Modafinil</t>
+  </si>
+  <si>
+    <t>Nintedanib,Tenecteplase</t>
+  </si>
+  <si>
+    <t>Cinacalcet,Citalopram,Azelastine,Rotigotine,Losartan,Progesterone,Olanzapine,Cyclobenzaprine,Perphenazine,Amitriptyline,Epinephrine,Desipramine,Ondansetron,Propranolol,Almotriptan,Asenapine,Pimozide,Ziprasidone,Imipramine,Clonidine,Modafinil,Clozapine|Cinacalcet,Citalopram,Azelastine,Rotigotine,Losartan,Progesterone,Olanzapine,Cyclobenzaprine,Perphenazine,Amitriptyline,Epinephrine,Desipramine,Ondansetron,Propranolol,Almotriptan,Asenapine,Pimozide,Ziprasidone,Imipramine,Clonidine,Modafinil,Clozapine|Dextromethorphan,Cinacalcet,Citalopram,Tiotropium,Ketamine,Cevimeline,Dronabinol,Histamine,Eletriptan,Azelastine,Oxycodone,Brompheniramine,Rotigotine,Diphenhydramine,Quetiapine,Oxymorphone,Losartan,Progesterone,Olanzapine,Cyclobenzaprine,Phenylephrine,Perphenazine,Oxybutynin,Zolmitriptan,Clemastine,Tizanidine,Tramadol,Fentanyl,Amitriptyline,Hydromorphone,Conivaptan,Mirabegron,Escitalopram,Dexamethasone,Frovatriptan,Aripiprazole,Trazodone,Paroxetine,Ondansetron,Darifenacin,Rizatriptan,Hydrocodone,Almotriptan,Codeine,Desipramine,Epinephrine,Propranolol,Sufentanil,Asenapine,Buspirone,Donepezil,Pimozide,Ziprasidone,Carbinoxamine,Ticagrelor,Imipramine,Clonidine,Ipratropium bromide,Modafinil,Salmeterol,Dopamine,Clozapine,Fluphenazine,Morphine</t>
+  </si>
+  <si>
+    <t>Cabergoline,Midodrine,Droxidopa,Iloprost,Quetiapine,Losartan,Nortriptyline,Loxapine,Olanzapine,Phenylephrine,Amitriptyline,Paliperidone,Mirabegron,Aripiprazole,Epinephrine,Nefazodone,Bromocriptine,Ergotamine,Oxymetazoline,Lisdexamfetamine,Terazosin,Ziprasidone,Dextroamphetamine,Doxepin,Trimipramine,Imipramine,Clonidine,Modafinil,Clozapine</t>
+  </si>
+  <si>
+    <t>Mirabegron,Olanzapine,Amitriptyline,Losartan</t>
+  </si>
+  <si>
+    <t>Cinacalcet,Propantheline,Citalopram,Cabergoline,Tiotropium,Cyclopentolate,Amoxapine,Cevimeline,Triptorelin,Histamine,Degarelix,Midodrine,Apraclonidine,Eletriptan,Azelastine,Pseudoephedrine,Cyproheptadine,Mirtazapine,Cetirizine,Brompheniramine,Ephedrine,Diphenhydramine,Quetiapine,Losartan,Acamprosate,Nortriptyline,Triprolidine,Olanzapine,Cyclobenzaprine,Isometheptene,Pergolide,Phenylephrine,Oxybutynin,Promethazine,Loxapine,Clemastine,Protirelin,Leuprolide,Tramadol,Amitriptyline,Paliperidone,Conivaptan,Pramipexole,Escitalopram,Aripiprazole,Trazodone,Desipramine,Epinephrine,Paroxetine,Darifenacin,Bromocriptine,Nefazodone,Scopolamine,Naphazoline,Ropinirole,Asenapine,Ergotamine,Donepezil,Lisdexamfetamine,Terazosin,Ziprasidone,Phentolamine,Dextroamphetamine,Carbinoxamine,Doxepin,Trimipramine,Imipramine,Droperidol,Clonidine,Maprotiline,Ipratropium bromide,Modafinil,Clozapine|Cinacalcet,Propantheline,Citalopram,Cabergoline,Tiotropium,Cyclopentolate,Amoxapine,Cevimeline,Triptorelin,Histamine,Degarelix,Midodrine,Apraclonidine,Eletriptan,Azelastine,Pseudoephedrine,Cyproheptadine,Mirtazapine,Cetirizine,Brompheniramine,Ephedrine,Diphenhydramine,Quetiapine,Losartan,Acamprosate,Nortriptyline,Triprolidine,Olanzapine,Cyclobenzaprine,Isometheptene,Pergolide,Phenylephrine,Oxybutynin,Promethazine,Loxapine,Clemastine,Protirelin,Leuprolide,Tramadol,Amitriptyline,Paliperidone,Conivaptan,Pramipexole,Dexamethasone,Escitalopram,Aripiprazole,Trazodone,Desipramine,Epinephrine,Paroxetine,Darifenacin,Bromocriptine,Nefazodone,Scopolamine,Naphazoline,Ropinirole,Asenapine,Bivalirudin,Ergotamine,Donepezil,Lisdexamfetamine,Terazosin,Ziprasidone,Phentolamine,Dextroamphetamine,Carbinoxamine,Doxepin,Trimipramine,Imipramine,Droperidol,Clonidine,Maprotiline,Ipratropium bromide,Modafinil,Clozapine</t>
+  </si>
+  <si>
+    <t>Indacaterol,Cabergoline,Tesamorelin,Adenosine,Amoxapine,Mefloquine,Histamine,Droxidopa,Timolol,Eletriptan,Pseudoephedrine,Iloprost,Teriparatide,Formoterol,Mirtazapine,Famotidine,Levodopa,Rotigotine,Quetiapine,Nortriptyline,Loxapine,Olanzapine,Lurasidone,Perphenazine,Metoprolol,Sotalol,Methamphetamine,Terbutaline,Amitriptyline,Paliperidone,Conivaptan,Pramipexole,Mirabegron,Aripiprazole,Epinephrine,Desipramine,Propranolol,Ondansetron,Ranitidine,Bromocriptine,Metipranolol,Metoclopramide,Ropinirole,Asenapine,Amphetamine,Ziprasidone,Dextroamphetamine,Arformoterol,Doxepin,Imipramine,Maprotiline,Regadenoson,Haloperidol,Salmeterol,Dopamine,Clozapine,Fluphenazine|Cinacalcet,Cevimeline,Midodrine,Apraclonidine,Ephedrine,Cyclobenzaprine,Protirelin,Oxybutynin,Clemastine,Succinylcholine,Trazodone,Epinephrine,Paroxetine,Bromocriptine,Ropinirole,Bivalirudin,Carbinoxamine,Citalopram,Amoxapine,Eletriptan,Pseudoephedrine,Mirtazapine,Quetiapine,Losartan,Isometheptene,Olanzapine,Phenylephrine,Loxapine,Paliperidone,Conivaptan,Pramipexole,Escitalopram,Aripiprazole,Nefazodone,Naphazoline,Phentolamine,Droperidol,Clonidine,Clozapine,Dicyclomine,Propantheline,Pilocarpine,Tiotropium,Azelastine,Cyproheptadine,Cetirizine,Diphenhydramine,Acamprosate,Triprolidine,Promethazine,Leuprolide,Tramadol,Amitriptyline,Hyoscyamine,Scopolamine,Metoclopramide,Asenapine,Ergotamine,Oxymetazoline,Donepezil,Terazosin,Trimipramine,Solifenacin,Ipratropium bromide,Haloperidol,Cabergoline,Cyclopentolate,Triptorelin,Histamine,Degarelix,Droxidopa,Brompheniramine,Nortriptyline,Pergolide,Lurasidone,Dexamethasone,Dihydroergotamine,Desipramine,Darifenacin,Atropine,Lisdexamfetamine,Ziprasidone,Dextroamphetamine,Doxepin,Imipramine,Maprotiline,Modafinil</t>
   </si>
   <si>
     <t>AKT1,ADCY1</t>
@@ -709,13 +709,13 @@
     <t>Isotretinoin</t>
   </si>
   <si>
-    <t>Fluoxetine,Ziprasidone,Zidovudine,Prasugrel,Testosterone,Tacrolimus,Propofol,Estradiol,Methotrexate,Lidocaine,Propafenone,Quetiapine,Olanzapine,Aripiprazole,Tofacitinib,Saquinavir,Valsartan,Warfarin</t>
-  </si>
-  <si>
-    <t>Ziprasidone,Prasugrel,Menthol,Gabapentin,Quetiapine,Olanzapine,Aripiprazole,Glycine,Pramipexole,Memantine|Ziprasidone,Quetiapine,Olanzapine,Aripiprazole</t>
-  </si>
-  <si>
-    <t>Betaxolol,Ziprasidone,Sotalol,Quetiapine,Olanzapine,Aripiprazole,Bisoprolol,Pramipexole,Arformoterol</t>
+    <t>Testosterone,Propafenone,Tofacitinib,Quetiapine,Ziprasidone,Aripiprazole,Warfarin,Tacrolimus,Olanzapine,Prasugrel,Fluoxetine,Methotrexate,Valsartan,Zidovudine,Lidocaine,Saquinavir,Estradiol,Propofol</t>
+  </si>
+  <si>
+    <t>Gabapentin,Pramipexole,Ziprasidone,Quetiapine,Aripiprazole,Glycine,Olanzapine,Prasugrel,Menthol,Memantine|Aripiprazole,Olanzapine,Ziprasidone,Quetiapine</t>
+  </si>
+  <si>
+    <t>Pramipexole,Ziprasidone,Betaxolol,Arformoterol,Quetiapine,Aripiprazole,Olanzapine,Bisoprolol,Sotalol</t>
   </si>
   <si>
     <t>CRABP2</t>
@@ -772,46 +772,46 @@
     <t>development of hyperlipidemia in acne patients treated with retinoic acid (RA)</t>
   </si>
   <si>
-    <t>Celecoxib,Nicardipine,Perphenazine</t>
-  </si>
-  <si>
-    <t>Enalaprilat,Ramipril,Enalapril,Fosinopril,Trandolapril,Captopril,Lisinopril,Quinapril,Benazepril</t>
-  </si>
-  <si>
-    <t>Ibuprofen,Diclofenac,Piroxicam,Naproxen,Ketoprofen,Celecoxib,Sulindac,Salicylic acid,Fenoprofen,Flurbiprofen,Diflunisal|Leuprolide,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Goserelin,Lisdexamfetamine,Pilocarpine,Eletriptan,Nicardipine,Phentolamine,Acamprosate,Nafarelin,Amoxapine,Epinephrine,Citalopram,Triptorelin,Amitriptyline,Bromocriptine,Imipramine,Irbesartan,Valsartan,Doxazosin,Dihydroergotamine,Dexamethasone,Clonidine,Telmisartan,Dextroamphetamine,Trazodone,Candesartan,Metoclopramide,Danazol,Maprotiline,Paroxetine,Mirtazapine,Aripiprazole,Olanzapine,Pseudoephedrine,Lurasidone,Cyclobenzaprine,Pramipexole,Diphenhydramine,Fenoldopam,Clomipramine,Atropine,Escitalopram,Phenylephrine,Trimipramine,Losartan,Donepezil,Olmesartan,Pergolide,Hydroxyzine,Nortriptyline,Disopyramide,Desipramine,Apomorphine,Histrelin</t>
+    <t>Nicardipine,Celecoxib,Perphenazine</t>
+  </si>
+  <si>
+    <t>Fosinopril,Trandolapril,Enalapril,Ramipril,Benazepril,Quinapril,Lisinopril,Captopril,Enalaprilat</t>
+  </si>
+  <si>
+    <t>Celecoxib,Diclofenac,Flurbiprofen,Piroxicam,Ibuprofen,Ketoprofen,Sulindac,Fenoprofen,Diflunisal,Naproxen,Salicylic acid|Citalopram,Pilocarpine,Danazol,Amoxapine,Triptorelin,Goserelin,Eletriptan,Doxazosin,Pseudoephedrine,Mirtazapine,Clomipramine,Apomorphine,Diphenhydramine,Losartan,Nortriptyline,Acamprosate,Olanzapine,Pergolide,Phenylephrine,Lurasidone,Candesartan,Cyclobenzaprine,Histrelin,Leuprolide,Tramadol,Amitriptyline,Fenoldopam,Pramipexole,Dexamethasone,Escitalopram,Olmesartan,Telmisartan,Aripiprazole,Risperidone,Irbesartan,Epinephrine,Desipramine,Trazodone,Paroxetine,Atropine,Dihydroergotamine,Nicardipine,Bromocriptine,Valsartan,Metoclopramide,Ropinirole,Tropicamide,Donepezil,Lisdexamfetamine,Phentolamine,Hydroxyzine,Dextroamphetamine,Trimipramine,Imipramine,Clonidine,Maprotiline,Disopyramide,Nafarelin,Clozapine</t>
   </si>
   <si>
     <t>Dasatinib</t>
   </si>
   <si>
-    <t>Fondaparinux sodium,Leuprolide,Heparin,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Goserelin,Lisdexamfetamine,Pilocarpine,Eletriptan,Nicardipine,Phentolamine,Acamprosate,Nafarelin,Amoxapine,Epinephrine,Citalopram,Triptorelin,Amitriptyline,Bromocriptine,Imipramine,Irbesartan,Valsartan,Doxazosin,Dihydroergotamine,Clonidine,Telmisartan,Dextroamphetamine,Trazodone,Candesartan,Metoclopramide,Danazol,Maprotiline,Paroxetine,Mirtazapine,Aripiprazole,Olanzapine,Pseudoephedrine,Lurasidone,Cyclobenzaprine,Pramipexole,Diphenhydramine,Fenoldopam,Clomipramine,Atropine,Escitalopram,Phenylephrine,Trimipramine,Losartan,Donepezil,Olmesartan,Pergolide,Tinzaparin,Hydroxyzine,Nortriptyline,Disopyramide,Desipramine,Apomorphine,Histrelin</t>
-  </si>
-  <si>
-    <t>Celecoxib,Dasatinib|Celecoxib,Dasatinib|Celecoxib,Amitriptyline,Dasatinib|Desflurane,Tacrolimus,Estradiol,Hyaluronidase,Methyltestosterone,Naloxone,Fluoxetine,Testosterone,Abiraterone,Celecoxib,Amitriptyline,Sulindac,Valsartan,Repaglinide,Diclofenac,Naproxen,Captopril,Ketoprofen,Olanzapine,Flurbiprofen,Clomipramine,Ibuprofen,Piroxicam,Losartan,Prednisone,Estrone,Salicylic acid,Fenoprofen,Nortriptyline,Diflunisal</t>
-  </si>
-  <si>
-    <t>Almotriptan,Ropinirole,Maraviroc,Risperidone,Clozapine,Tropicamide,Tramadol,Adenosine,Zolmitriptan,Naloxone,Frovatriptan,Pilocarpine,Eletriptan,Nicardipine,Progesterone,Nalbuphine,Levodopa,Amphetamine,Amoxapine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pindolol,Dexamethasone,Pentazocine,Rizatriptan,Octreotide,Trazodone,Ketoprofen,Metoclopramide,Maprotiline,Paroxetine,Mirtazapine,Aripiprazole,Olanzapine,Lurasidone,Perphenazine,Pramipexole,Pasireotide,Memantine,Sumatriptan,Diphenhydramine,Naratriptan,Atropine,Trimipramine,Propranolol,Menthol,Pergolide,Tinzaparin,Gabapentin,Nortriptyline,Disopyramide,Desipramine,Apomorphine</t>
-  </si>
-  <si>
-    <t>Epinephrine,Propranolol|Almotriptan,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Zolmitriptan,Naloxone,Frovatriptan,Eletriptan,Nicardipine,Nalbuphine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pentazocine,Rizatriptan,Maprotiline,Paroxetine,Olanzapine,Aripiprazole,Pramipexole,Sumatriptan,Naratriptan,Atropine,Trimipramine,Pergolide,Nortriptyline,Desipramine,Apomorphine|Ropinirole,Risperidone,Clozapine,Goserelin,Adenosine,Eletriptan,Amoxapine,Epinephrine,Amitriptyline,Bromocriptine,Imipramine,Pindolol,Dextroamphetamine,Metoclopramide,Maprotiline,Pseudoephedrine,Aripiprazole,Mirtazapine,Olanzapine,Lurasidone,Perphenazine,Pramipexole,Fenoldopam,Propranolol,Pergolide,Nortriptyline,Desipramine,Apomorphine|Aripiprazole,Clomipramine,Desipramine,Ropinirole,Trimipramine,Risperidone,Amoxapine,Clozapine,Trazodone,Pergolide,Maprotiline,Mirtazapine,Bromocriptine,Olanzapine,Imipramine,Nortriptyline,Amitriptyline,Pramipexole,Apomorphine</t>
-  </si>
-  <si>
-    <t>Almotriptan,Maraviroc,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Adenosine,Zolmitriptan,Naloxone,Frovatriptan,Pilocarpine,Eletriptan,Nicardipine,Progesterone,Nalbuphine,Amoxapine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pindolol,Dexamethasone,Pentazocine,Rizatriptan,Trazodone,Ketoprofen,Metoclopramide,Paroxetine,Maprotiline,Olanzapine,Aripiprazole,Mirtazapine,Lurasidone,Perphenazine,Pasireotide,Pramipexole,Sumatriptan,Diphenhydramine,Memantine,Naratriptan,Atropine,Trimipramine,Propranolol,Menthol,Pergolide,Gabapentin,Tinzaparin,Apomorphine,Nortriptyline,Disopyramide,Desipramine,Octreotide|Almotriptan,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Zolmitriptan,Naloxone,Frovatriptan,Eletriptan,Nicardipine,Nalbuphine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pentazocine,Rizatriptan,Maprotiline,Paroxetine,Olanzapine,Aripiprazole,Pramipexole,Sumatriptan,Naratriptan,Atropine,Trimipramine,Pergolide,Nortriptyline,Desipramine,Apomorphine</t>
-  </si>
-  <si>
-    <t>Epinephrine,Pseudoephedrine</t>
-  </si>
-  <si>
-    <t>Almotriptan,Maraviroc,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Adenosine,Zolmitriptan,Naloxone,Frovatriptan,Pilocarpine,Eletriptan,Nicardipine,Progesterone,Nalbuphine,Amoxapine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pindolol,Dexamethasone,Pentazocine,Rizatriptan,Trazodone,Ketoprofen,Metoclopramide,Paroxetine,Maprotiline,Olanzapine,Aripiprazole,Mirtazapine,Lurasidone,Perphenazine,Pasireotide,Pramipexole,Sumatriptan,Diphenhydramine,Memantine,Naratriptan,Atropine,Trimipramine,Propranolol,Menthol,Pergolide,Gabapentin,Tinzaparin,Apomorphine,Nortriptyline,Disopyramide,Desipramine,Octreotide|Almotriptan,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Zolmitriptan,Naloxone,Frovatriptan,Eletriptan,Nicardipine,Nalbuphine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pentazocine,Rizatriptan,Maprotiline,Paroxetine,Olanzapine,Aripiprazole,Pramipexole,Sumatriptan,Naratriptan,Atropine,Trimipramine,Pergolide,Nortriptyline,Desipramine,Apomorphine|Almotriptan,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Zolmitriptan,Naloxone,Frovatriptan,Eletriptan,Nicardipine,Nalbuphine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pentazocine,Rizatriptan,Maprotiline,Paroxetine,Olanzapine,Aripiprazole,Pramipexole,Sumatriptan,Naratriptan,Atropine,Trimipramine,Pergolide,Nortriptyline,Desipramine,Apomorphine|Aripiprazole,Clomipramine,Desipramine,Ropinirole,Trimipramine,Risperidone,Amoxapine,Clozapine,Trazodone,Pergolide,Maprotiline,Mirtazapine,Bromocriptine,Olanzapine,Imipramine,Nortriptyline,Amitriptyline,Pramipexole,Apomorphine</t>
-  </si>
-  <si>
-    <t>Desflurane,Risperidone,Clozapine,Tacrolimus,Estradiol,Hyaluronidase,Methyltestosterone,Naloxone,Lisdexamfetamine,Fluoxetine,Nicardipine,Testosterone,Abiraterone,Epinephrine,Celecoxib,Amitriptyline,Bromocriptine,Sulindac,Imipramine,Valsartan,Doxazosin,Clonidine,Repaglinide,Diclofenac,Naproxen,Captopril,Dextroamphetamine,Ketoprofen,Olanzapine,Aripiprazole,Flurbiprofen,Fenoldopam,Clomipramine,Ibuprofen,Piroxicam,Phenylephrine,Trimipramine,Losartan,Prednisone,Estrone,Pergolide,Salicylic acid,Fenoprofen,Nortriptyline,Disopyramide,Diflunisal</t>
+    <t>Citalopram,Pilocarpine,Danazol,Amoxapine,Triptorelin,Goserelin,Heparin,Eletriptan,Doxazosin,Pseudoephedrine,Mirtazapine,Clomipramine,Apomorphine,Diphenhydramine,Losartan,Nortriptyline,Acamprosate,Olanzapine,Pergolide,Phenylephrine,Lurasidone,Candesartan,Cyclobenzaprine,Histrelin,Leuprolide,Tramadol,Amitriptyline,Fenoldopam,Pramipexole,Olmesartan,Fondaparinux sodium,Escitalopram,Telmisartan,Aripiprazole,Risperidone,Irbesartan,Epinephrine,Desipramine,Trazodone,Paroxetine,Atropine,Dihydroergotamine,Nicardipine,Bromocriptine,Valsartan,Metoclopramide,Ropinirole,Tropicamide,Donepezil,Lisdexamfetamine,Phentolamine,Hydroxyzine,Dextroamphetamine,Trimipramine,Imipramine,Clonidine,Tinzaparin,Maprotiline,Disopyramide,Nafarelin,Clozapine</t>
+  </si>
+  <si>
+    <t>Celecoxib,Dasatinib|Celecoxib,Dasatinib|Celecoxib,Amitriptyline,Dasatinib|Testosterone,Flurbiprofen,Diclofenac,Piroxicam,Hyaluronidase,Methyltestosterone,Fluoxetine,Prednisone,Diflunisal,Estradiol,Clomipramine,Abiraterone,Losartan,Tacrolimus,Nortriptyline,Olanzapine,Repaglinide,Sulindac,Naproxen,Estrone,Salicylic acid,Amitriptyline,Ibuprofen,Ketoprofen,Fenoprofen,Captopril,Valsartan,Celecoxib,Desflurane,Naloxone</t>
+  </si>
+  <si>
+    <t>Pilocarpine,Sumatriptan,Adenosine,Amoxapine,Eletriptan,Mirtazapine,Levodopa,Apomorphine,Gabapentin,Pindolol,Diphenhydramine,Pentazocine,Nortriptyline,Progesterone,Olanzapine,Pergolide,Lurasidone,Perphenazine,Zolmitriptan,Tramadol,Amitriptyline,Fentanyl,Pramipexole,Dexamethasone,Maraviroc,Frovatriptan,Aripiprazole,Risperidone,Trazodone,Desipramine,Paroxetine,Propranolol,Atropine,Ketoprofen,Nicardipine,Almotriptan,Rizatriptan,Dihydroergotamine,Metoclopramide,Pasireotide,Bromocriptine,Ropinirole,Tropicamide,Octreotide,Nalbuphine,Amphetamine,Naloxone,Trimipramine,Imipramine,Naratriptan,Tinzaparin,Maprotiline,Disopyramide,Menthol,Clozapine,Memantine</t>
+  </si>
+  <si>
+    <t>Epinephrine,Propranolol|Sumatriptan,Eletriptan,Apomorphine,Pentazocine,Nortriptyline,Olanzapine,Pergolide,Zolmitriptan,Tramadol,Amitriptyline,Fentanyl,Pramipexole,Frovatriptan,Aripiprazole,Risperidone,Dihydroergotamine,Paroxetine,Desipramine,Rizatriptan,Atropine,Bromocriptine,Nicardipine,Almotriptan,Ropinirole,Tropicamide,Nalbuphine,Naloxone,Imipramine,Trimipramine,Naratriptan,Maprotiline,Clozapine|Adenosine,Amoxapine,Goserelin,Eletriptan,Pseudoephedrine,Mirtazapine,Apomorphine,Pindolol,Nortriptyline,Olanzapine,Pergolide,Lurasidone,Perphenazine,Amitriptyline,Fenoldopam,Pramipexole,Aripiprazole,Risperidone,Epinephrine,Propranolol,Desipramine,Bromocriptine,Metoclopramide,Ropinirole,Dextroamphetamine,Imipramine,Maprotiline,Clozapine|Amitriptyline,Apomorphine,Pramipexole,Aripiprazole,Risperidone,Nortriptyline,Imipramine,Trazodone,Amoxapine,Clozapine,Desipramine,Bromocriptine,Olanzapine,Trimipramine,Pergolide,Maprotiline,Ropinirole,Mirtazapine,Clomipramine</t>
+  </si>
+  <si>
+    <t>Pilocarpine,Sumatriptan,Adenosine,Amoxapine,Eletriptan,Mirtazapine,Apomorphine,Gabapentin,Pindolol,Diphenhydramine,Rizatriptan,Nortriptyline,Pentazocine,Progesterone,Olanzapine,Pergolide,Lurasidone,Perphenazine,Zolmitriptan,Tramadol,Fentanyl,Amitriptyline,Pramipexole,Dexamethasone,Maraviroc,Frovatriptan,Aripiprazole,Risperidone,Dihydroergotamine,Paroxetine,Trazodone,Desipramine,Atropine,Bromocriptine,Nicardipine,Almotriptan,Propranolol,Ketoprofen,Metoclopramide,Pasireotide,Ropinirole,Tropicamide,Octreotide,Nalbuphine,Naloxone,Imipramine,Trimipramine,Naratriptan,Tinzaparin,Maprotiline,Disopyramide,Menthol,Clozapine,Memantine|Sumatriptan,Eletriptan,Apomorphine,Pentazocine,Nortriptyline,Olanzapine,Pergolide,Zolmitriptan,Tramadol,Amitriptyline,Fentanyl,Pramipexole,Frovatriptan,Aripiprazole,Risperidone,Dihydroergotamine,Paroxetine,Desipramine,Rizatriptan,Atropine,Bromocriptine,Nicardipine,Almotriptan,Ropinirole,Tropicamide,Nalbuphine,Naloxone,Imipramine,Trimipramine,Naratriptan,Maprotiline,Clozapine</t>
+  </si>
+  <si>
+    <t>Pseudoephedrine,Epinephrine</t>
+  </si>
+  <si>
+    <t>Pilocarpine,Sumatriptan,Adenosine,Amoxapine,Eletriptan,Mirtazapine,Apomorphine,Gabapentin,Pindolol,Diphenhydramine,Rizatriptan,Nortriptyline,Pentazocine,Progesterone,Olanzapine,Pergolide,Lurasidone,Perphenazine,Zolmitriptan,Tramadol,Fentanyl,Amitriptyline,Pramipexole,Dexamethasone,Maraviroc,Frovatriptan,Aripiprazole,Risperidone,Dihydroergotamine,Paroxetine,Trazodone,Desipramine,Atropine,Bromocriptine,Nicardipine,Almotriptan,Propranolol,Ketoprofen,Metoclopramide,Pasireotide,Ropinirole,Tropicamide,Octreotide,Nalbuphine,Naloxone,Imipramine,Trimipramine,Naratriptan,Tinzaparin,Maprotiline,Disopyramide,Menthol,Clozapine,Memantine|Sumatriptan,Eletriptan,Apomorphine,Pentazocine,Nortriptyline,Olanzapine,Pergolide,Zolmitriptan,Tramadol,Amitriptyline,Fentanyl,Pramipexole,Frovatriptan,Aripiprazole,Risperidone,Dihydroergotamine,Paroxetine,Desipramine,Rizatriptan,Atropine,Bromocriptine,Nicardipine,Almotriptan,Ropinirole,Tropicamide,Nalbuphine,Naloxone,Imipramine,Trimipramine,Naratriptan,Maprotiline,Clozapine|Sumatriptan,Eletriptan,Apomorphine,Pentazocine,Nortriptyline,Olanzapine,Pergolide,Zolmitriptan,Tramadol,Amitriptyline,Fentanyl,Pramipexole,Frovatriptan,Aripiprazole,Risperidone,Dihydroergotamine,Paroxetine,Desipramine,Rizatriptan,Atropine,Bromocriptine,Nicardipine,Almotriptan,Ropinirole,Tropicamide,Nalbuphine,Naloxone,Imipramine,Trimipramine,Naratriptan,Maprotiline,Clozapine|Amitriptyline,Apomorphine,Pramipexole,Aripiprazole,Risperidone,Nortriptyline,Imipramine,Trazodone,Amoxapine,Clozapine,Desipramine,Bromocriptine,Olanzapine,Trimipramine,Pergolide,Maprotiline,Ropinirole,Mirtazapine,Clomipramine</t>
+  </si>
+  <si>
+    <t>Testosterone,Flurbiprofen,Diclofenac,Piroxicam,Hyaluronidase,Methyltestosterone,Fluoxetine,Prednisone,Diflunisal,Doxazosin,Estradiol,Clomipramine,Abiraterone,Losartan,Tacrolimus,Nortriptyline,Olanzapine,Phenylephrine,Repaglinide,Pergolide,Sulindac,Naproxen,Estrone,Salicylic acid,Amitriptyline,Fenoldopam,Aripiprazole,Risperidone,Epinephrine,Ibuprofen,Ketoprofen,Fenoprofen,Captopril,Nicardipine,Bromocriptine,Valsartan,Lisdexamfetamine,Celecoxib,Dextroamphetamine,Desflurane,Naloxone,Imipramine,Trimipramine,Clonidine,Disopyramide,Clozapine</t>
   </si>
   <si>
     <t>Sulindac,Dasatinib|Dasatinib|Dasatinib</t>
   </si>
   <si>
-    <t>Clozapine,Tropicamide,Insulin Human,Pilocarpine,Nicardipine,Epinephrine,Amitriptyline,Imipramine,Pindolol,Maprotiline,Paroxetine,Pseudoephedrine,Aripiprazole,Mirtazapine,Olanzapine,Diphenhydramine,Ibuprofen,Atropine,Propranolol,Nortriptyline,Disopyramide,Desipramine</t>
+    <t>Pilocarpine,Pseudoephedrine,Mirtazapine,Pindolol,Diphenhydramine,Nortriptyline,Olanzapine,Insulin Human,Amitriptyline,Aripiprazole,Epinephrine,Paroxetine,Desipramine,Propranolol,Atropine,Ibuprofen,Nicardipine,Tropicamide,Imipramine,Maprotiline,Disopyramide,Clozapine</t>
   </si>
   <si>
     <t>Insulin Human</t>
@@ -820,13 +820,13 @@
     <t>Celecoxib</t>
   </si>
   <si>
-    <t>Almotriptan,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Zolmitriptan,Naloxone,Frovatriptan,Pilocarpine,Eletriptan,Nicardipine,Nalbuphine,Levodopa,Amphetamine,Amoxapine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pindolol,Dexamethasone,Pentazocine,Rizatriptan,Trazodone,Ketoprofen,Metoclopramide,Paroxetine,Maprotiline,Olanzapine,Mirtazapine,Aripiprazole,Lurasidone,Perphenazine,Pramipexole,Diphenhydramine,Sumatriptan,Naratriptan,Atropine,Trimipramine,Propranolol,Pergolide,Nortriptyline,Disopyramide,Desipramine,Apomorphine</t>
-  </si>
-  <si>
-    <t>Tenecteplase,Alteplase,Tranexamic Acid,Aprotinin</t>
-  </si>
-  <si>
-    <t>Almotriptan,Maraviroc,Ropinirole,Risperidone,Clozapine,Tropicamide,Tramadol,Adenosine,Zolmitriptan,Naloxone,Frovatriptan,Pilocarpine,Eletriptan,Nicardipine,Progesterone,Nalbuphine,Amoxapine,Amitriptyline,Bromocriptine,Imipramine,Fentanyl,Dihydroergotamine,Pindolol,Dexamethasone,Pentazocine,Rizatriptan,Trazodone,Ketoprofen,Metoclopramide,Paroxetine,Maprotiline,Olanzapine,Aripiprazole,Mirtazapine,Lurasidone,Perphenazine,Pasireotide,Pramipexole,Sumatriptan,Diphenhydramine,Memantine,Naratriptan,Atropine,Trimipramine,Propranolol,Menthol,Pergolide,Gabapentin,Tinzaparin,Apomorphine,Nortriptyline,Disopyramide,Desipramine,Octreotide</t>
+    <t>Pilocarpine,Sumatriptan,Amoxapine,Eletriptan,Mirtazapine,Levodopa,Apomorphine,Pindolol,Diphenhydramine,Nortriptyline,Pentazocine,Olanzapine,Pergolide,Lurasidone,Perphenazine,Zolmitriptan,Tramadol,Fentanyl,Amitriptyline,Pramipexole,Dexamethasone,Frovatriptan,Aripiprazole,Risperidone,Dihydroergotamine,Propranolol,Paroxetine,Desipramine,Atropine,Bromocriptine,Nicardipine,Almotriptan,Trazodone,Rizatriptan,Metoclopramide,Ketoprofen,Ropinirole,Tropicamide,Nalbuphine,Amphetamine,Naloxone,Imipramine,Trimipramine,Naratriptan,Maprotiline,Disopyramide,Clozapine</t>
+  </si>
+  <si>
+    <t>Aprotinin,Alteplase,Tranexamic Acid,Tenecteplase</t>
+  </si>
+  <si>
+    <t>Pilocarpine,Sumatriptan,Adenosine,Amoxapine,Eletriptan,Mirtazapine,Apomorphine,Gabapentin,Pindolol,Diphenhydramine,Rizatriptan,Nortriptyline,Pentazocine,Progesterone,Olanzapine,Pergolide,Lurasidone,Perphenazine,Zolmitriptan,Tramadol,Fentanyl,Amitriptyline,Pramipexole,Dexamethasone,Maraviroc,Frovatriptan,Aripiprazole,Risperidone,Dihydroergotamine,Paroxetine,Trazodone,Desipramine,Atropine,Bromocriptine,Nicardipine,Almotriptan,Propranolol,Ketoprofen,Metoclopramide,Pasireotide,Ropinirole,Tropicamide,Octreotide,Nalbuphine,Naloxone,Imipramine,Trimipramine,Naratriptan,Tinzaparin,Maprotiline,Disopyramide,Menthol,Clozapine,Memantine</t>
   </si>
   <si>
     <t>REN</t>
@@ -1075,13 +1075,13 @@
     <t>Blocking of CB1 receptor with rimonabant improves cardiac functions in the early and late stages after MI, decreases arterial stiffness and reduces cardiac remodelling</t>
   </si>
   <si>
-    <t>Lidocaine,Erlotinib</t>
+    <t>Erlotinib,Lidocaine</t>
   </si>
   <si>
     <t>Acitretin</t>
   </si>
   <si>
-    <t>Fluoxetine,Phenytoin,Zidovudine,Erlotinib,Prednisone,Abiraterone,Fosphenytoin,Acitretin,Rosuvastatin,Saquinavir</t>
+    <t>Abiraterone,Fluoxetine,Prednisone,Zidovudine,Acitretin,Saquinavir,Phenytoin,Erlotinib,Rosuvastatin,Fosphenytoin</t>
   </si>
   <si>
     <t>ADRB2</t>
@@ -1111,19 +1111,19 @@
     <t>Review article postulating whether resveratrol can be a treatment for myopathies.</t>
   </si>
   <si>
-    <t>Indomethacin,Sulindac</t>
-  </si>
-  <si>
-    <t>Probenecid,Erlotinib,Tacrolimus,Acitretin,Tetracycline,Hyaluronidase,Sulindac,Indomethacin,Insulin Detemir|Erlotinib,Trastuzumab emtansine,Lidocaine,Trastuzumab,Pertuzumab</t>
-  </si>
-  <si>
-    <t>Trastuzumab,Lidocaine,Erlotinib</t>
-  </si>
-  <si>
-    <t>Vemurafenib,Probenecid,Erlotinib,Tacrolimus,Acitretin,Tetracycline,Hyaluronidase,Sulindac,Indomethacin,Insulin Detemir,Sulfamethizole</t>
-  </si>
-  <si>
-    <t>Erlotinib,Trastuzumab emtansine,Lidocaine,Trastuzumab,Pertuzumab</t>
+    <t>Sulindac,Indomethacin</t>
+  </si>
+  <si>
+    <t>Tetracycline,Tacrolimus,Hyaluronidase,Sulindac,Indomethacin,Insulin Detemir,Acitretin,Probenecid,Erlotinib|Pertuzumab,Trastuzumab,Lidocaine,Erlotinib,Trastuzumab emtansine</t>
+  </si>
+  <si>
+    <t>Erlotinib,Trastuzumab,Lidocaine</t>
+  </si>
+  <si>
+    <t>Sulfamethizole,Tetracycline,Tacrolimus,Vemurafenib,Hyaluronidase,Sulindac,Indomethacin,Insulin Detemir,Acitretin,Probenecid,Erlotinib</t>
+  </si>
+  <si>
+    <t>Pertuzumab,Trastuzumab,Lidocaine,Erlotinib,Trastuzumab emtansine</t>
   </si>
   <si>
     <t>ATM,PIK3CA</t>
@@ -1174,22 +1174,22 @@
     <t>Sorafenib induces neuropathic pain.</t>
   </si>
   <si>
-    <t>Clonidine,Aripiprazole,Hydroflumethiazide,Erythromycin,Hydrochlorothiazide,Risperidone,Erlotinib,Prazosin,Clozapine,Pergolide,Ketoprofen,Quetiapine,Olanzapine,Droxidopa,Fenoprofen,Sulindac,Naloxone,Valsartan,Vandetanib</t>
-  </si>
-  <si>
-    <t>Capsaicin,Thalidomide,Ketoprofen,Sulindac,Fenoprofen|Clonidine,Aripiprazole,Acamprosate,Erythromycin,Atropine,Ropinirole,Risperidone,Prazosin,Clozapine,Pergolide,Paroxetine,Quetiapine,Mirtazapine,Droxidopa,Olanzapine,Valsartan,Pramipexole,Pilocarpine|Sulfasalazine,Thalidomide</t>
-  </si>
-  <si>
-    <t>Aripiprazole,Atropine,Erlotinib,Blinatumomab,Propranolol,Clozapine,Paroxetine,Quetiapine,Mirtazapine,Droxidopa,Olanzapine,Vandetanib,Pilocarpine</t>
-  </si>
-  <si>
-    <t>Ropinirole,Risperidone,Prazosin,Diphenoxylate,Clozapine,Tramadol,Naloxone,Pilocarpine,Acamprosate,Erythromycin,Amoxapine,Citalopram,Droxidopa,Valsartan,Dexamethasone,Clonidine,Eprosartan,Pentazocine,Telmisartan,Naltrexone,Candesartan,Ketoprofen,Paroxetine,Danazol,Quetiapine,Mirtazapine,Aripiprazole,Olanzapine,Pramipexole,Memantine,Pasireotide,Lanreotide,Atropine,Donepezil,Olmesartan,Losartan,Propranolol,Menthol,Pergolide,Gabapentin,Morphine,Octreotide</t>
-  </si>
-  <si>
-    <t>Lanreotide,Atropine,Ropinirole,Risperidone,Propranolol,Clozapine,Diphenoxylate,Menthol,Pergolide,Ketoprofen,Paroxetine,Quetiapine,Gabapentin,Mirtazapine,Aripiprazole,Olanzapine,Naloxone,Pramipexole,Octreotide,Pilocarpine|Lanreotide,Atropine,Ropinirole,Risperidone,Propranolol,Clozapine,Diphenoxylate,Menthol,Pergolide,Ketoprofen,Paroxetine,Quetiapine,Gabapentin,Mirtazapine,Aripiprazole,Olanzapine,Naloxone,Pramipexole,Octreotide,Pilocarpine</t>
-  </si>
-  <si>
-    <t>Ropinirole,Risperidone,Clozapine,Tramadol,Riluzole,Naloxone,Pilocarpine,Erythromycin,Citalopram,Sulindac,Dexamethasone,Clonidine,Paroxetine,Danazol,Quetiapine,Mirtazapine,Aripiprazole,Atropine,Donepezil,Losartan,Propranolol,Pergolide,Morphine</t>
+    <t>Quetiapine,Aripiprazole,Risperidone,Naloxone,Olanzapine,Pergolide,Clonidine,Hydrochlorothiazide,Vandetanib,Fenoprofen,Ketoprofen,Prazosin,Droxidopa,Valsartan,Erythromycin,Sulindac,Hydroflumethiazide,Erlotinib,Clozapine</t>
+  </si>
+  <si>
+    <t>Thalidomide,Ketoprofen,Fenoprofen,Sulindac,Capsaicin|Pramipexole,Quetiapine,Pilocarpine,Aripiprazole,Risperidone,Acamprosate,Olanzapine,Paroxetine,Pergolide,Clonidine,Atropine,Droxidopa,Valsartan,Erythromycin,Ropinirole,Prazosin,Clozapine,Mirtazapine|Sulfasalazine,Thalidomide</t>
+  </si>
+  <si>
+    <t>Pilocarpine,Quetiapine,Aripiprazole,Olanzapine,Paroxetine,Propranolol,Vandetanib,Blinatumomab,Atropine,Droxidopa,Erlotinib,Clozapine,Mirtazapine</t>
+  </si>
+  <si>
+    <t>Citalopram,Pilocarpine,Danazol,Amoxapine,Droxidopa,Diphenoxylate,Prazosin,Mirtazapine,Gabapentin,Quetiapine,Losartan,Acamprosate,Pentazocine,Olanzapine,Pergolide,Lanreotide,Candesartan,Erythromycin,Tramadol,Olmesartan,Pramipexole,Dexamethasone,Telmisartan,Aripiprazole,Risperidone,Paroxetine,Propranolol,Ketoprofen,Atropine,Morphine,Valsartan,Pasireotide,Ropinirole,Naltrexone,Octreotide,Donepezil,Naloxone,Clonidine,Eprosartan,Menthol,Clozapine,Memantine</t>
+  </si>
+  <si>
+    <t>Octreotide,Gabapentin,Pramipexole,Pilocarpine,Quetiapine,Aripiprazole,Risperidone,Naloxone,Olanzapine,Propranolol,Paroxetine,Pergolide,Atropine,Lanreotide,Ketoprofen,Menthol,Diphenoxylate,Ropinirole,Clozapine,Mirtazapine|Octreotide,Gabapentin,Pramipexole,Pilocarpine,Quetiapine,Aripiprazole,Risperidone,Naloxone,Olanzapine,Propranolol,Paroxetine,Pergolide,Atropine,Lanreotide,Ketoprofen,Menthol,Diphenoxylate,Ropinirole,Clozapine,Mirtazapine</t>
+  </si>
+  <si>
+    <t>Citalopram,Pilocarpine,Danazol,Riluzole,Mirtazapine,Quetiapine,Losartan,Pergolide,Sulindac,Erythromycin,Tramadol,Dexamethasone,Aripiprazole,Risperidone,Paroxetine,Propranolol,Atropine,Ropinirole,Donepezil,Naloxone,Clonidine,Clozapine,Morphine</t>
   </si>
   <si>
     <t>TP53,EDNRA,NFKBIA</t>
@@ -1240,7 +1240,7 @@
     <t>Glutathione levels were decreased in a pnacreatitis model.</t>
   </si>
   <si>
-    <t>Ziprasidone,Aripiprazole,Doxepin,Levodopa,Risperidone,Amoxapine,Clozapine,Loxapine,Asenapine,Fluphenazine,Iloperidone,Metoclopramide,Quetiapine,Olanzapine,Mirtazapine,Amitriptyline,Apomorphine,Perphenazine,Pramipexole,Treprostinil</t>
+    <t>Amitriptyline,Apomorphine,Levodopa,Pramipexole,Ziprasidone,Quetiapine,Aripiprazole,Risperidone,Loxapine,Olanzapine,Treprostinil,Iloperidone,Perphenazine,Amoxapine,Doxepin,Metoclopramide,Clozapine,Asenapine,Fluphenazine,Mirtazapine</t>
   </si>
   <si>
     <t>Ibuprofen</t>
@@ -1252,10 +1252,10 @@
     <t>Basiliximab,Etanercept</t>
   </si>
   <si>
-    <t>Ziprasidone,Aripiprazole,Doxepin,Clozapine,Promethazine,Loxapine,Asenapine,Paroxetine,Quetiapine,Tiotropium,Amitriptyline,Olanzapine,Mirtazapine,Trihexyphenidyl</t>
-  </si>
-  <si>
-    <t>Ibuprofen|Ziprasidone,Trifluoperazine,Risperidone,Clozapine,Loxapine,Tramadol,Amoxapine,Tiotropium,Amitriptyline,Dexamethasone,Pimavanserin,Metoclopramide,Paroxetine,Nefazodone,Quetiapine,Olanzapine,Mirtazapine,Aripiprazole,Pramipexole,Doxepin,Promethazine,Asenapine,Iloperidone,Trihexyphenidyl,Apomorphine</t>
+    <t>Ziprasidone,Quetiapine,Tiotropium,Aripiprazole,Doxepin,Loxapine,Olanzapine,Paroxetine,Promethazine,Clozapine,Trihexyphenidyl,Mirtazapine,Asenapine,Amitriptyline</t>
+  </si>
+  <si>
+    <t>Ibuprofen|Tiotropium,Amoxapine,Trihexyphenidyl,Mirtazapine,Apomorphine,Quetiapine,Loxapine,Olanzapine,Promethazine,Tramadol,Iloperidone,Amitriptyline,Pramipexole,Dexamethasone,Aripiprazole,Risperidone,Paroxetine,Nefazodone,Pimavanserin,Metoclopramide,Asenapine,Ziprasidone,Doxepin,Trifluoperazine,Clozapine</t>
   </si>
   <si>
     <t>ADORA2B</t>
@@ -1330,10 +1330,10 @@
     <t>Celecoxib,Dasatinib</t>
   </si>
   <si>
-    <t>Benazepril,Trandolapril,Ramipril,Captopril</t>
-  </si>
-  <si>
-    <t>Ibuprofen,Vandetanib</t>
+    <t>Captopril,Benazepril,Trandolapril,Ramipril</t>
+  </si>
+  <si>
+    <t>Vandetanib,Ibuprofen</t>
   </si>
   <si>
     <t>Vandetanib|Dasatinib|Dasatinib</t>
@@ -1420,10 +1420,10 @@
     <t>Prior therapy caused proteinuria in a single patient case study.</t>
   </si>
   <si>
-    <t>Paroxetine,Cocaine,Atropine</t>
-  </si>
-  <si>
-    <t>Paroxetine,Atropine|Atropine,Ropinirole,Cocaine,Paroxetine,Goserelin,Cevimeline,Pramipexole</t>
+    <t>Atropine,Paroxetine,Cocaine</t>
+  </si>
+  <si>
+    <t>Atropine,Paroxetine|Pramipexole,Paroxetine,Cevimeline,Atropine,Goserelin,Cocaine,Ropinirole</t>
   </si>
   <si>
     <t>Canakinumab</t>
@@ -1432,16 +1432,16 @@
     <t>Sulfasalazine</t>
   </si>
   <si>
-    <t>Atropine,Ropinirole,Cocaine,Paroxetine,Goserelin,Cevimeline,Pramipexole</t>
-  </si>
-  <si>
-    <t>Paroxetine,Cocaine,Atropine|Atropine,Ropinirole,Cocaine,Paroxetine,Goserelin,Cevimeline,Pramipexole</t>
-  </si>
-  <si>
-    <t>Tofacitinib,Ibrutinib,Memantine,Abatacept</t>
-  </si>
-  <si>
-    <t>Atropine,Ropinirole,Cocaine,Paroxetine,Goserelin,Cevimeline,Pramipexole|Paroxetine,Atropine</t>
+    <t>Pramipexole,Paroxetine,Cevimeline,Atropine,Goserelin,Cocaine,Ropinirole</t>
+  </si>
+  <si>
+    <t>Atropine,Paroxetine,Cocaine|Pramipexole,Paroxetine,Cevimeline,Atropine,Goserelin,Cocaine,Ropinirole</t>
+  </si>
+  <si>
+    <t>Abatacept,Ibrutinib,Tofacitinib,Memantine</t>
+  </si>
+  <si>
+    <t>Pramipexole,Paroxetine,Cevimeline,Atropine,Goserelin,Cocaine,Ropinirole|Atropine,Paroxetine</t>
   </si>
   <si>
     <t>Ibrutinib</t>
@@ -1450,10 +1450,10 @@
     <t>Sulfasalazine|Tofacitinib</t>
   </si>
   <si>
-    <t>Paroxetine,Cocaine,Atropine|Tofacitinib,Abatacept</t>
-  </si>
-  <si>
-    <t>Paroxetine,Cocaine,Atropine|Paroxetine,Atropine</t>
+    <t>Atropine,Paroxetine,Cocaine|Abatacept,Tofacitinib</t>
+  </si>
+  <si>
+    <t>Atropine,Paroxetine,Cocaine|Atropine,Paroxetine</t>
   </si>
   <si>
     <t>HRH4,ADRA1D</t>
@@ -1705,7 +1705,7 @@
     <t>ART-123 is a safe intervention in critically ill patients with sepsis and suspected disseminated intravascular coagulation. The study provided evidence suggestive of efficacy supporting further development of this drug in sepsis-associated coagulopathy</t>
   </si>
   <si>
-    <t>Abciximab,Tirofiban,Bosutinib,Ponatinib,Nintedanib,Dasatinib</t>
+    <t>Bosutinib,Nintedanib,Tirofiban,Ponatinib,Dasatinib,Abciximab</t>
   </si>
   <si>
     <t>Bosutinib,Imatinib</t>

</xml_diff>